<commit_message>
Add tests for Journals Purchase Form
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C798632
</commit_message>
<xml_diff>
--- a/PPIUK-Phase2/PPIUK-Research/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Phase2/PPIUK-Research/src/test/resources/CobaltUsers.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19770" windowHeight="8475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0" calcOnSave="0" concurrentCalc="0"/>
+  <oleSize ref="A1:R26"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="282">
   <si>
     <t>UserName</t>
   </si>
@@ -844,13 +845,32 @@
   </si>
   <si>
     <t>Global_page111!</t>
+  </si>
+  <si>
+    <t>tr-journals-purchase-form@yandex.com</t>
+  </si>
+  <si>
+    <t>Minsk2016Research</t>
+  </si>
+  <si>
+    <t>ci-tr-journals-purchase-form@yandex.com</t>
+  </si>
+  <si>
+    <t>Security answer</t>
+  </si>
+  <si>
+    <t>Thomson Reuters</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,7 +1040,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1055,7 +1075,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1266,18 +1286,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A87" sqref="A86:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3454,27 +3474,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>202</v>
       </c>
@@ -3482,12 +3506,34 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>204</v>
       </c>
       <c r="B3" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add users for research and update purchase form test
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C799419
</commit_message>
<xml_diff>
--- a/PPIUK-Phase2/PPIUK-Research/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Phase2/PPIUK-Research/src/test/resources/CobaltUsers.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19770" windowHeight="8475" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19770" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0" concurrentCalc="0"/>
-  <oleSize ref="A1:R26"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="312">
   <si>
     <t>UserName</t>
   </si>
@@ -860,6 +859,96 @@
   </si>
   <si>
     <t>Thomson Reuters</t>
+  </si>
+  <si>
+    <t>PLResearchUser1</t>
+  </si>
+  <si>
+    <t>PLResearchUser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>PLResearch</t>
+  </si>
+  <si>
+    <t>PLResearchUser2</t>
+  </si>
+  <si>
+    <t>PLResearchUser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser2</t>
+  </si>
+  <si>
+    <t>PLResearchUser3</t>
+  </si>
+  <si>
+    <t>PLResearchUser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser3</t>
+  </si>
+  <si>
+    <t>PLResearchUser4</t>
+  </si>
+  <si>
+    <t>PLResearchUser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser4</t>
+  </si>
+  <si>
+    <t>PLResearchUser5</t>
+  </si>
+  <si>
+    <t>PLResearchUser5@mailinator.com</t>
+  </si>
+  <si>
+    <t>TestUser5</t>
+  </si>
+  <si>
+    <t>PLResearchUser6</t>
+  </si>
+  <si>
+    <t>PLResearchUser6@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser6</t>
+  </si>
+  <si>
+    <t>PLResearchUser7</t>
+  </si>
+  <si>
+    <t>PLResearchUser7@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser7</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PLResearchUser8</t>
+  </si>
+  <si>
+    <t>PLResearchUser8@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser8</t>
+  </si>
+  <si>
+    <t>PLResearchUser9</t>
+  </si>
+  <si>
+    <t>PLResearchUser9@mailinator.com</t>
+  </si>
+  <si>
+    <t>ResearchUser9</t>
   </si>
   <si>
     <t>Y</t>
@@ -966,7 +1055,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -979,6 +1068,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1284,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A87" sqref="A86:A87"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,9 +1390,10 @@
     <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1322,8 +1415,14 @@
       <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1443,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1363,7 +1462,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1382,7 +1481,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1403,7 +1502,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +1523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1445,7 +1544,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +1565,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>273</v>
       </c>
@@ -1485,7 +1584,7 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1506,7 +1605,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1527,7 +1626,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1647,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1668,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1588,7 +1687,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1609,7 +1708,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -3354,7 +3453,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>267</v>
       </c>
@@ -3371,7 +3470,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>269</v>
       </c>
@@ -3386,6 +3485,213 @@
       </c>
       <c r="G114" s="10" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>281</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="H115" t="s">
+        <v>283</v>
+      </c>
+      <c r="I115" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>285</v>
+      </c>
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H116" t="s">
+        <v>287</v>
+      </c>
+      <c r="I116" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>288</v>
+      </c>
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G117" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I117" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>291</v>
+      </c>
+      <c r="B118" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G118" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H118" t="s">
+        <v>293</v>
+      </c>
+      <c r="I118" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>294</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G119" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="H119" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="I119" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>297</v>
+      </c>
+      <c r="B120" t="s">
+        <v>52</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G120" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H120" t="s">
+        <v>299</v>
+      </c>
+      <c r="I120" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>300</v>
+      </c>
+      <c r="B121" t="s">
+        <v>52</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G121" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="H121" t="s">
+        <v>302</v>
+      </c>
+      <c r="I121" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>305</v>
+      </c>
+      <c r="B122" t="s">
+        <v>52</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G122" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="H122" t="s">
+        <v>307</v>
+      </c>
+      <c r="I122" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>308</v>
+      </c>
+      <c r="B123" t="s">
+        <v>52</v>
+      </c>
+      <c r="E123" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F123" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G123" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="H123" t="s">
+        <v>310</v>
+      </c>
+      <c r="I123" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3466,9 +3772,18 @@
     <hyperlink ref="G111" r:id="rId74"/>
     <hyperlink ref="G114" r:id="rId75"/>
     <hyperlink ref="G112" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G119" r:id="rId77"/>
+    <hyperlink ref="G115" r:id="rId78"/>
+    <hyperlink ref="G116" r:id="rId79"/>
+    <hyperlink ref="G117" r:id="rId80"/>
+    <hyperlink ref="G118" r:id="rId81"/>
+    <hyperlink ref="G120" r:id="rId82"/>
+    <hyperlink ref="G121" r:id="rId83"/>
+    <hyperlink ref="G122" r:id="rId84"/>
+    <hyperlink ref="G123" r:id="rId85"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId86"/>
 </worksheet>
 </file>
 
@@ -3476,7 +3791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>